<commit_message>
Moved jacks closer to board edge
</commit_message>
<xml_diff>
--- a/CameraTriggerR2PCB/CameraTriggerR2MouserBOM.xlsx
+++ b/CameraTriggerR2PCB/CameraTriggerR2MouserBOM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="166">
   <si>
     <t>Reference</t>
   </si>
@@ -289,223 +289,229 @@
     <t>660-MF1/4DCT26A1001F</t>
   </si>
   <si>
+    <t xml:space="preserve">LM7805CT </t>
+  </si>
+  <si>
+    <t>TI</t>
+  </si>
+  <si>
+    <t>926-LM7805CT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80-ESL107M016AC3AA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESL107M016AC3AA </t>
+  </si>
+  <si>
+    <t>kmet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESL106M100AE3AA </t>
+  </si>
+  <si>
+    <t>kimet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80-ESL106M100AE3AA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">610-PN2222A </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central Semiconductor </t>
+  </si>
+  <si>
+    <t>Adafruit</t>
+  </si>
+  <si>
+    <t>Feather M0</t>
+  </si>
+  <si>
+    <t>490-SJ1-2503A</t>
+  </si>
+  <si>
+    <t>SJ1-2503A</t>
+  </si>
+  <si>
+    <t>2.5 mm Camera Jack</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBR10U45SD1-T </t>
+  </si>
+  <si>
+    <t xml:space="preserve">621-SBR10U45SD1-T </t>
+  </si>
+  <si>
+    <t>Diodes Incorporated</t>
+  </si>
+  <si>
+    <t>DO-201AD-2</t>
+  </si>
+  <si>
+    <t>Avago</t>
+  </si>
+  <si>
+    <t>HLMP-1790</t>
+  </si>
+  <si>
+    <t>630-HLMP-1790</t>
+  </si>
+  <si>
+    <t>1k</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>J12</t>
+  </si>
+  <si>
+    <t>Adafruit Bluefruit LE SPI Friend - Bluetooth Low Energy (BLE)</t>
+  </si>
+  <si>
+    <t>U7</t>
+  </si>
+  <si>
+    <t>Connector_PinHeader_2.54mm:PinHeader_1x09_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t>ILD74</t>
+  </si>
+  <si>
+    <t>782-ILD74</t>
+  </si>
+  <si>
+    <t>Vishay</t>
+  </si>
+  <si>
+    <t>485-3178</t>
+  </si>
+  <si>
+    <t xml:space="preserve">485-2633 </t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>15K</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>660-MF1/4LCT52R510G</t>
+  </si>
+  <si>
+    <t>MF1/4LCT52R510G</t>
+  </si>
+  <si>
+    <t>HLMP-K150</t>
+  </si>
+  <si>
+    <t>630-HLMP-K150</t>
+  </si>
+  <si>
+    <t>PWR</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>amass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XT30U-M </t>
+  </si>
+  <si>
+    <t>https://www.tme.eu/Document/3cbfa5cfa544d79584972dd5234a409e/XT30U%20SPEC.pdf</t>
+  </si>
+  <si>
+    <t>TLHK46Q1R2</t>
+  </si>
+  <si>
+    <t>78-TLHK46Q1R2</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
+    <t>Focus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">485-2886 </t>
+  </si>
+  <si>
+    <t>603-MF0207FTE52-14K7</t>
+  </si>
+  <si>
+    <t>HLMP-LG71-XZ0DD</t>
+  </si>
+  <si>
+    <t>J13</t>
+  </si>
+  <si>
+    <t>J14</t>
+  </si>
+  <si>
+    <t>5V on</t>
+  </si>
+  <si>
+    <t>Pwr sw</t>
+  </si>
+  <si>
+    <t>S103M47Z5UN63J7R</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>0.01 uf</t>
+  </si>
+  <si>
+    <t>594-S103M47Z5UN63J7R</t>
+  </si>
+  <si>
+    <t>Capacitor_THT:C_Disc_D7.5mm_W2.5mm_P5.00mm</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>AS11CB</t>
+  </si>
+  <si>
     <t>NKK</t>
   </si>
   <si>
-    <t xml:space="preserve">LM7805CT </t>
-  </si>
-  <si>
-    <t>TI</t>
-  </si>
-  <si>
-    <t>926-LM7805CT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80-ESL107M016AC3AA </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ESL107M016AC3AA </t>
-  </si>
-  <si>
-    <t>kmet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ESL106M100AE3AA </t>
-  </si>
-  <si>
-    <t>kimet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80-ESL106M100AE3AA </t>
-  </si>
-  <si>
-    <t xml:space="preserve">610-PN2222A </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Central Semiconductor </t>
-  </si>
-  <si>
-    <t>Adafruit</t>
-  </si>
-  <si>
-    <t>633-AS11BH</t>
-  </si>
-  <si>
-    <t>AS11BH</t>
-  </si>
-  <si>
-    <t>Feather M0</t>
-  </si>
-  <si>
-    <t>490-SJ1-2503A</t>
-  </si>
-  <si>
-    <t>SJ1-2503A</t>
-  </si>
-  <si>
-    <t>2.5 mm Camera Jack</t>
-  </si>
-  <si>
-    <t>D3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SBR10U45SD1-T </t>
-  </si>
-  <si>
-    <t xml:space="preserve">621-SBR10U45SD1-T </t>
-  </si>
-  <si>
-    <t>Diodes Incorporated</t>
-  </si>
-  <si>
-    <t>DO-201AD-2</t>
-  </si>
-  <si>
-    <t>Avago</t>
-  </si>
-  <si>
-    <t>HLMP-1790</t>
-  </si>
-  <si>
-    <t>630-HLMP-1790</t>
-  </si>
-  <si>
-    <t>1k</t>
-  </si>
-  <si>
-    <t>Q2</t>
-  </si>
-  <si>
-    <t>Q3</t>
-  </si>
-  <si>
-    <t>U6</t>
-  </si>
-  <si>
-    <t>J12</t>
-  </si>
-  <si>
-    <t>Adafruit Bluefruit LE SPI Friend - Bluetooth Low Energy (BLE)</t>
-  </si>
-  <si>
-    <t>U7</t>
-  </si>
-  <si>
-    <t>Connector_PinHeader_2.54mm:PinHeader_1x09_P2.54mm_Vertical</t>
-  </si>
-  <si>
-    <t>ILD74</t>
-  </si>
-  <si>
-    <t>782-ILD74</t>
-  </si>
-  <si>
-    <t>Vishay</t>
-  </si>
-  <si>
-    <t>485-3178</t>
-  </si>
-  <si>
-    <t xml:space="preserve">485-2633 </t>
-  </si>
-  <si>
-    <t>R7</t>
-  </si>
-  <si>
-    <t>R8</t>
-  </si>
-  <si>
-    <t>15K</t>
-  </si>
-  <si>
-    <t>R4</t>
-  </si>
-  <si>
-    <t>R6</t>
-  </si>
-  <si>
-    <t>660-MF1/4LCT52R510G</t>
-  </si>
-  <si>
-    <t>MF1/4LCT52R510G</t>
-  </si>
-  <si>
-    <t>HLMP-K150</t>
-  </si>
-  <si>
-    <t>630-HLMP-K150</t>
-  </si>
-  <si>
-    <t>PWR</t>
-  </si>
-  <si>
-    <t>D4</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>amass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XT30U-M </t>
-  </si>
-  <si>
-    <t>https://www.tme.eu/Document/3cbfa5cfa544d79584972dd5234a409e/XT30U%20SPEC.pdf</t>
-  </si>
-  <si>
-    <t>TLHK46Q1R2</t>
-  </si>
-  <si>
-    <t>78-TLHK46Q1R2</t>
-  </si>
-  <si>
-    <t>D5</t>
-  </si>
-  <si>
-    <t>Focus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">485-2886 </t>
-  </si>
-  <si>
-    <t>603-MF0207FTE52-14K7</t>
-  </si>
-  <si>
-    <t>HLMP-LG71-XZ0DD</t>
-  </si>
-  <si>
-    <t>J13</t>
-  </si>
-  <si>
-    <t>J14</t>
-  </si>
-  <si>
-    <t>5V on</t>
-  </si>
-  <si>
-    <t>Pwr sw</t>
-  </si>
-  <si>
-    <t>S103M47Z5UN63J7R</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
-    <t>C4</t>
-  </si>
-  <si>
-    <t>0.01 uf</t>
-  </si>
-  <si>
-    <t>594-S103M47Z5UN63J7R</t>
-  </si>
-  <si>
-    <t>Capacitor_THT:C_Disc_D7.5mm_W2.5mm_P5.00mm</t>
+    <t>633-AS11CB</t>
+  </si>
+  <si>
+    <t>IC1</t>
   </si>
 </sst>
 </file>
@@ -1333,10 +1339,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1399,13 +1405,13 @@
         <v>59</v>
       </c>
       <c r="D3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" t="s">
         <v>96</v>
       </c>
-      <c r="E3" t="s">
-        <v>97</v>
-      </c>
       <c r="F3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G3" t="s">
         <v>28</v>
@@ -1422,13 +1428,13 @@
         <v>59</v>
       </c>
       <c r="D4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E4" t="s">
         <v>98</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>99</v>
-      </c>
-      <c r="F4" t="s">
-        <v>100</v>
       </c>
       <c r="G4" t="s">
         <v>28</v>
@@ -1442,16 +1448,16 @@
         <v>27</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="G5" t="s">
         <v>28</v>
@@ -1465,16 +1471,16 @@
         <v>45</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D6" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F6" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="G6" t="s">
         <v>28</v>
@@ -1482,50 +1488,50 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D7" t="s">
+        <v>108</v>
+      </c>
+      <c r="E7" t="s">
         <v>110</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="F7" t="s">
+        <v>109</v>
+      </c>
+      <c r="G7" t="s">
         <v>111</v>
-      </c>
-      <c r="E7" t="s">
-        <v>113</v>
-      </c>
-      <c r="F7" t="s">
-        <v>112</v>
-      </c>
-      <c r="G7" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D8" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E8" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F8" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
+        <v>145</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F9" t="s">
         <v>149</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="F9" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1536,13 +1542,13 @@
         <v>63</v>
       </c>
       <c r="D10" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E10" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="G10" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30">
@@ -1559,10 +1565,10 @@
         <v>2886</v>
       </c>
       <c r="E11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F11" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="G11" t="s">
         <v>28</v>
@@ -1570,27 +1576,27 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D12" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E12" t="s">
         <v>78</v>
       </c>
       <c r="F12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30">
       <c r="A13" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>6</v>
@@ -1607,10 +1613,10 @@
     </row>
     <row r="14" spans="1:7" ht="30">
       <c r="A14" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>6</v>
@@ -1800,10 +1806,10 @@
         <v>49</v>
       </c>
       <c r="E22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G22" t="s">
         <v>51</v>
@@ -1811,7 +1817,7 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>49</v>
@@ -1823,10 +1829,10 @@
         <v>49</v>
       </c>
       <c r="E23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G23" t="s">
         <v>51</v>
@@ -1834,7 +1840,7 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>49</v>
@@ -1846,10 +1852,10 @@
         <v>49</v>
       </c>
       <c r="E24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G24" t="s">
         <v>51</v>
@@ -1883,7 +1889,7 @@
         <v>36</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>31</v>
@@ -1926,7 +1932,7 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B28" s="2">
         <v>220</v>
@@ -1957,7 +1963,7 @@
     </row>
     <row r="30" spans="1:7" ht="30">
       <c r="A30" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B30" s="2">
         <v>51</v>
@@ -1966,18 +1972,18 @@
         <v>31</v>
       </c>
       <c r="D30" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E30" t="s">
         <v>87</v>
       </c>
       <c r="F30" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="30">
       <c r="A31" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B31" s="2">
         <v>51</v>
@@ -1986,27 +1992,27 @@
         <v>31</v>
       </c>
       <c r="D31" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E31" t="s">
         <v>87</v>
       </c>
       <c r="F31" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="30">
       <c r="A32" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F32" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="30">
@@ -2020,13 +2026,13 @@
         <v>66</v>
       </c>
       <c r="D33" t="s">
-        <v>105</v>
+        <v>162</v>
       </c>
       <c r="E33" t="s">
-        <v>91</v>
+        <v>163</v>
       </c>
       <c r="F33" t="s">
-        <v>104</v>
+        <v>164</v>
       </c>
       <c r="G33" t="s">
         <v>28</v>
@@ -2112,13 +2118,13 @@
         <v>69</v>
       </c>
       <c r="D37" t="s">
+        <v>91</v>
+      </c>
+      <c r="E37" t="s">
         <v>92</v>
       </c>
-      <c r="E37" t="s">
+      <c r="F37" t="s">
         <v>93</v>
-      </c>
-      <c r="F37" t="s">
-        <v>94</v>
       </c>
       <c r="G37" t="s">
         <v>70</v>
@@ -2129,19 +2135,19 @@
         <v>23</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D38" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E38" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F38" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G38" t="s">
         <v>25</v>
@@ -2152,19 +2158,19 @@
         <v>55</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D39" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E39" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F39" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G39" t="s">
         <v>25</v>
@@ -2172,79 +2178,119 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>121</v>
+        <v>165</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D40">
         <v>3178</v>
       </c>
       <c r="E40" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F40" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="30">
       <c r="A41" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D41">
         <v>2633</v>
       </c>
       <c r="E41" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F41" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="G41" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
+        <v>155</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>163</v>
-      </c>
       <c r="D42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E42" t="s">
+        <v>124</v>
+      </c>
+      <c r="F42" t="s">
         <v>158</v>
-      </c>
-      <c r="E42" t="s">
-        <v>128</v>
-      </c>
-      <c r="F42" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" t="s">
+        <v>156</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D43" t="s">
+        <v>154</v>
+      </c>
+      <c r="E43" t="s">
+        <v>124</v>
+      </c>
+      <c r="F43" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" t="s">
         <v>160</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B44" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D44" t="s">
+        <v>154</v>
+      </c>
+      <c r="E44" t="s">
+        <v>124</v>
+      </c>
+      <c r="F44" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" t="s">
         <v>161</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="D43" t="s">
+      <c r="B45" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D45" t="s">
+        <v>154</v>
+      </c>
+      <c r="E45" t="s">
+        <v>124</v>
+      </c>
+      <c r="F45" t="s">
         <v>158</v>
-      </c>
-      <c r="E43" t="s">
-        <v>128</v>
-      </c>
-      <c r="F43" t="s">
-        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>